<commit_message>
Users Api code & input data for GET,POST,DELETE & Authorization
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/InputData_Users.xlsx
+++ b/src/test/resources/TestData/InputData_Users.xlsx
@@ -3,15 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{709E10E2-0C6D-4991-98E3-93A839CE60FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{291B9862-FDC4-40EC-84A1-B437D28B6CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17328" windowHeight="13224" xr2:uid="{C6FDCADB-182C-446E-8512-FF2F915DDD3D}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17376" windowHeight="13224" activeTab="3" xr2:uid="{C6FDCADB-182C-446E-8512-FF2F915DDD3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Users_Authorization" sheetId="1" r:id="rId1"/>
+    <sheet name="InputData_User_GET" sheetId="2" r:id="rId2"/>
+    <sheet name="InputData_Users_POST" sheetId="3" r:id="rId3"/>
+    <sheet name="InputData_Users_DELETE" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:P5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
   <si>
     <t>To Check Authorization with valid username and password</t>
   </si>
@@ -63,13 +66,181 @@
   </si>
   <si>
     <t>Unauthorized Access</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Users_ID</t>
+  </si>
+  <si>
+    <t>GET method for Valid UsersID</t>
+  </si>
+  <si>
+    <t>U01</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>GET method for non existing UserID</t>
+  </si>
+  <si>
+    <t>U2021</t>
+  </si>
+  <si>
+    <t>User Not Found</t>
+  </si>
+  <si>
+    <t>GET method for invalid UserID</t>
+  </si>
+  <si>
+    <t>ABC01</t>
+  </si>
+  <si>
+    <t>GET method for  UsersID with special character</t>
+  </si>
+  <si>
+    <t>US@03</t>
+  </si>
+  <si>
+    <t>GET method for  UsersID with decimal</t>
+  </si>
+  <si>
+    <t>GET method for  UsersID as blank</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>phone_number</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>time_zone</t>
+  </si>
+  <si>
+    <t>linkedin_url</t>
+  </si>
+  <si>
+    <t>education_ug</t>
+  </si>
+  <si>
+    <t>education_pg</t>
+  </si>
+  <si>
+    <t>visa_status</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>Sam Dsouza</t>
+  </si>
+  <si>
+    <t>Raleigh</t>
+  </si>
+  <si>
+    <t>EST</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/Sam Dsouza/</t>
+  </si>
+  <si>
+    <t>bsc</t>
+  </si>
+  <si>
+    <t>msc</t>
+  </si>
+  <si>
+    <t>H1B</t>
+  </si>
+  <si>
+    <t>today is a great day</t>
+  </si>
+  <si>
+    <t>Successfully Created</t>
+  </si>
+  <si>
+    <t>Failed to create - invalid data</t>
+  </si>
+  <si>
+    <t>h4-ead</t>
+  </si>
+  <si>
+    <t>www.linkedn.com</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Failed to create - missing either first or last names</t>
+  </si>
+  <si>
+    <t>Samantha Ben</t>
+  </si>
+  <si>
+    <t>New jersey</t>
+  </si>
+  <si>
+    <t>H4-EAD</t>
+  </si>
+  <si>
+    <t>abcdef</t>
+  </si>
+  <si>
+    <t>Failed to update-missing mandatory fields</t>
+  </si>
+  <si>
+    <t>IST</t>
+  </si>
+  <si>
+    <t>123rit</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>To delete an existing user id</t>
+  </si>
+  <si>
+    <t>User record successfully deleted</t>
+  </si>
+  <si>
+    <t>To delete where user id is invalid</t>
+  </si>
+  <si>
+    <t>U321</t>
+  </si>
+  <si>
+    <t>Failed to delete-user not found</t>
+  </si>
+  <si>
+    <t>To delete where user id is decimal</t>
+  </si>
+  <si>
+    <t>U4.3</t>
+  </si>
+  <si>
+    <t>To delete where user id has special character</t>
+  </si>
+  <si>
+    <t>U#01</t>
+  </si>
+  <si>
+    <t>To delete where user id is blank</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +258,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -130,20 +308,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{9643B2BD-F27D-43E6-9FB4-2BCDE806C99E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -457,7 +645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E5D993-1318-44A6-B297-253F91D40622}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -553,4 +741,424 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098C77B3-114A-4F69-8B1F-C591FE6D8C6E}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>404</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>404</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5">
+        <v>404</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>108.8</v>
+      </c>
+      <c r="C6">
+        <v>404</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>404</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{9AA997EC-53F8-4EE0-B37E-AFD7E8B867C3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB14EC7-31C3-4DA8-B024-B0776F7243D4}">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2">
+        <v>8764532198</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2">
+        <v>201</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>45678934</v>
+      </c>
+      <c r="J3">
+        <v>400</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4">
+        <v>400</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5">
+        <v>400</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>345.789649</v>
+      </c>
+      <c r="J6">
+        <v>400</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <v>400</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J8">
+        <v>400</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9">
+        <v>400</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10">
+        <v>6785489390</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s">
+        <v>53</v>
+      </c>
+      <c r="I10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10">
+        <v>400</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J11">
+        <v>400</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12">
+        <v>400</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FCB78B-9444-4B3D-8B47-723F4D1D04E1}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="6">
+        <v>200</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="6">
+        <v>404</v>
+      </c>
+      <c r="D3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="6">
+        <v>404</v>
+      </c>
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="6">
+        <v>404</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6">
+        <v>404</v>
+      </c>
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed the API constant name for users & userskills
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/InputData_Users.xlsx
+++ b/src/test/resources/TestData/InputData_Users.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{291B9862-FDC4-40EC-84A1-B437D28B6CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{83205F7D-090D-459D-A2C2-F775B3EE6EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17376" windowHeight="13224" activeTab="3" xr2:uid="{C6FDCADB-182C-446E-8512-FF2F915DDD3D}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17400" windowHeight="13224" activeTab="1" xr2:uid="{C6FDCADB-182C-446E-8512-FF2F915DDD3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Users_Authorization" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="InputData_Users_DELETE" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:P5"/>
+  <oleSize ref="A1:P24"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="68">
   <si>
     <t>To Check Authorization with valid username and password</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>U01</t>
-  </si>
-  <si>
-    <t>OK</t>
   </si>
   <si>
     <t>GET method for non existing UserID</t>
@@ -747,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098C77B3-114A-4F69-8B1F-C591FE6D8C6E}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -777,55 +774,52 @@
       <c r="C2">
         <v>200</v>
       </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
       </c>
       <c r="C3">
         <v>404</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
         <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
       </c>
       <c r="C4">
         <v>404</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C5">
         <v>404</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>108.8</v>
@@ -834,18 +828,18 @@
         <v>404</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7">
         <v>404</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -868,31 +862,31 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="J1" t="s">
         <v>11</v>
@@ -903,37 +897,37 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>8764532198</v>
       </c>
       <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>39</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>41</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>42</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>43</v>
-      </c>
-      <c r="I2" t="s">
-        <v>44</v>
       </c>
       <c r="J2">
         <v>201</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -944,29 +938,29 @@
         <v>400</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J4">
         <v>400</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J5">
         <v>400</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -977,7 +971,7 @@
         <v>400</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -985,83 +979,83 @@
         <v>400</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J8">
         <v>400</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J9">
         <v>400</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10">
         <v>6785489390</v>
       </c>
       <c r="C10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" t="s">
         <v>52</v>
       </c>
-      <c r="D10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>53</v>
-      </c>
-      <c r="I10" t="s">
-        <v>54</v>
       </c>
       <c r="J10">
         <v>400</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J11">
         <v>400</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J12">
         <v>400</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1073,7 +1067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FCB78B-9444-4B3D-8B47-723F4D1D04E1}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
@@ -1084,7 +1078,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>11</v>
@@ -1095,67 +1089,67 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="6">
         <v>200</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="C3" s="6">
         <v>404</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="C4" s="6">
         <v>404</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
         <v>66</v>
-      </c>
-      <c r="B5" t="s">
-        <v>67</v>
       </c>
       <c r="C5" s="6">
         <v>404</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6">
         <v>404</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Input data for POST Users and Skillmaster updated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/InputData_Users.xlsx
+++ b/src/test/resources/TestData/InputData_Users.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{193750AA-7FCE-4D27-AE5E-90BCD076E1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="19836" windowHeight="11220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="13440" windowHeight="5055" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Users_Authorization" sheetId="1" r:id="rId1"/>
@@ -21,16 +20,15 @@
     <sheet name="visa_status_POST" sheetId="11" r:id="rId11"/>
     <sheet name="comments_POST" sheetId="12" r:id="rId12"/>
     <sheet name="Invalid_Content" sheetId="13" r:id="rId13"/>
-    <sheet name="Text_POST" sheetId="14" r:id="rId14"/>
-    <sheet name="InputData_Users_PUT" sheetId="15" r:id="rId15"/>
+    <sheet name="InputData_Users_PUT" sheetId="15" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
   <oleSize ref="A14:F24"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="174">
   <si>
     <t>SCENARIO</t>
   </si>
@@ -495,18 +493,6 @@
   </si>
   <si>
     <t>Connecticut</t>
-  </si>
-  <si>
-    <t>bvis</t>
-  </si>
-  <si>
-    <t>mvis</t>
-  </si>
-  <si>
-    <t>details of a user</t>
-  </si>
-  <si>
-    <t>Failed to create-missing mandatory fields</t>
   </si>
   <si>
     <t>Update the record with valid data</t>
@@ -569,11 +555,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0;[Red]0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -590,13 +580,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -605,22 +588,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -658,8 +625,144 @@
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -672,8 +775,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -696,44 +985,283 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -743,31 +1271,73 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="Normal 2" xfId="32"/>
+    <cellStyle name="20% - Accent5" xfId="33" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="34" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="35" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="36" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="38" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="39" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="40" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="41" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="42" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="43" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="44" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="45" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="46" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="47" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="48" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="49" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1025,26 +1595,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="47.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.21875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="47.2190476190476" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.66666666666667" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.2190476190476" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" ht="15.75" spans="1:5">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -1061,7 +1631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8">
+    <row r="2" ht="30.75" spans="1:5">
       <c r="A2" s="22" t="s">
         <v>5</v>
       </c>
@@ -1072,7 +1642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8">
+    <row r="3" ht="30.75" spans="1:5">
       <c r="A3" s="22" t="s">
         <v>7</v>
       </c>
@@ -1089,7 +1659,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8">
+    <row r="4" ht="30.75" spans="1:5">
       <c r="A4" s="22" t="s">
         <v>10</v>
       </c>
@@ -1106,7 +1676,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8">
+    <row r="5" ht="30.75" spans="1:4">
       <c r="A5" s="22" t="s">
         <v>13</v>
       </c>
@@ -1122,29 +1692,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C3" r:id="rId1" display="2xx@Success"/>
+    <hyperlink ref="C4" r:id="rId2" display="New@2022"/>
+    <hyperlink ref="C5" r:id="rId1" display="2xx@Success"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="13" max="13" width="35.33203125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="35.3333333333333" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="10" customFormat="1">
+    <row r="1" s="10" customFormat="1" spans="1:13">
       <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
@@ -1183,7 +1755,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="86.4">
+    <row r="2" ht="105" spans="1:13">
       <c r="A2" s="12" t="s">
         <v>151</v>
       </c>
@@ -1220,26 +1792,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" tooltip="https://www.linkedin.com/in/apple bees/" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="G2" r:id="rId1" display="https://www.linkedin.com/in/apple bees/" tooltip="https://www.linkedin.com/in/apple bees/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="13" max="13" width="31.109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="31.1047619047619" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="10" customFormat="1">
+    <row r="1" s="10" customFormat="1" spans="1:13">
       <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
@@ -1278,7 +1852,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="86.4">
+    <row r="2" ht="105" spans="1:13">
       <c r="A2" s="12" t="s">
         <v>151</v>
       </c>
@@ -1315,27 +1889,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" tooltip="https://www.linkedin.com/in/apple bees/" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="G2" r:id="rId1" display="https://www.linkedin.com/in/apple bees/" tooltip="https://www.linkedin.com/in/apple bees/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="25.8857142857143" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.4380952380952" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="10" customFormat="1">
+    <row r="1" s="10" customFormat="1" spans="1:13">
       <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
@@ -1374,7 +1950,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="43.2">
+    <row r="2" ht="45" spans="1:13">
       <c r="A2" s="12" t="s">
         <v>151</v>
       </c>
@@ -1411,26 +1987,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" tooltip="https://www.linkedin.com/in/apple bees/" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="G2" r:id="rId1" display="https://www.linkedin.com/in/apple bees/" tooltip="https://www.linkedin.com/in/apple bees/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="13" max="13" width="27.5546875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="27.552380952381" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="10" customFormat="1">
+    <row r="1" s="10" customFormat="1" spans="1:13">
       <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
@@ -1452,7 +2030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="86.4">
+    <row r="2" ht="105" spans="1:13">
       <c r="A2" s="12" t="s">
         <v>151</v>
       </c>
@@ -1466,128 +2044,25 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:M2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="19.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.33203125" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="10" customFormat="1">
-      <c r="A1" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="72">
-      <c r="A2" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="C2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" t="s">
-        <v>155</v>
-      </c>
-      <c r="I2" t="s">
-        <v>156</v>
-      </c>
-      <c r="J2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" t="s">
-        <v>157</v>
-      </c>
-      <c r="L2">
-        <v>400</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>158</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" tooltip="https://www.linkedin.com/in/apple bees/" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="11.6640625"/>
+    <col min="4" max="4" width="11.6666666666667"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="28.8">
+    <row r="1" s="1" customFormat="1" ht="30" spans="1:13">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -1628,48 +2103,48 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" ht="67.95" customHeight="1">
+    <row r="2" s="2" customFormat="1" ht="67.95" customHeight="1" spans="1:13">
       <c r="A2" s="5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D2" s="7">
         <v>4569213584</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>42</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>46</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="L2" s="5">
         <v>201</v>
       </c>
       <c r="M2" s="5"/>
     </row>
-    <row r="3" spans="1:13" s="2" customFormat="1" ht="100.8">
+    <row r="3" s="2" customFormat="1" ht="105" spans="1:13">
       <c r="A3" s="9" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -1685,12 +2160,12 @@
         <v>400</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" s="2" customFormat="1" ht="403.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" s="2" customFormat="1" ht="409.5" spans="1:13">
       <c r="A4" s="9" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -1706,12 +2181,12 @@
         <v>400</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="2" customFormat="1" ht="288">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" s="2" customFormat="1" ht="330" spans="1:13">
       <c r="A5" s="9" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -1727,12 +2202,12 @@
         <v>400</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="2" customFormat="1" ht="150">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="1" ht="150" spans="1:13">
       <c r="A6" s="9" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -1748,12 +2223,12 @@
         <v>400</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="2" customFormat="1" ht="195">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" s="2" customFormat="1" ht="195" spans="1:13">
       <c r="A7" s="9" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -1769,12 +2244,12 @@
         <v>400</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" s="2" customFormat="1" ht="345">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" s="2" customFormat="1" ht="360" spans="1:13">
       <c r="A8" s="9" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -1790,12 +2265,12 @@
         <v>400</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="2" customFormat="1" ht="60">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" s="2" customFormat="1" ht="60" spans="1:13">
       <c r="A9" s="9" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -1811,12 +2286,12 @@
         <v>400</v>
       </c>
       <c r="M9" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" s="2" customFormat="1" ht="75" spans="1:13">
+      <c r="A10" s="9" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" s="2" customFormat="1" ht="75">
-      <c r="A10" s="9" t="s">
-        <v>177</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -1832,29 +2307,31 @@
         <v>400</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="G2" r:id="rId1" display="https://www.linkedin.com/in/DaveWilliam"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.1047619047619" customWidth="1"/>
+    <col min="2" max="2" width="8.33333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1871,7 +2348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1951,38 +2428,40 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B5" r:id="rId1" display="US@03"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="53.88671875" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="53.8857142857143" customWidth="1"/>
+    <col min="2" max="2" width="17.6666666666667" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="24.109375" customWidth="1"/>
+    <col min="4" max="4" width="24.1047619047619" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" customWidth="1"/>
-    <col min="7" max="7" width="39.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" customWidth="1"/>
-    <col min="11" max="11" width="24.33203125" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" customWidth="1"/>
-    <col min="13" max="13" width="31.88671875" customWidth="1"/>
+    <col min="6" max="6" width="10.4380952380952" customWidth="1"/>
+    <col min="7" max="7" width="39.6666666666667" customWidth="1"/>
+    <col min="8" max="8" width="16.4380952380952" customWidth="1"/>
+    <col min="9" max="9" width="17.3333333333333" customWidth="1"/>
+    <col min="10" max="10" width="12.3333333333333" customWidth="1"/>
+    <col min="11" max="11" width="24.3333333333333" customWidth="1"/>
+    <col min="12" max="12" width="10.1047619047619" customWidth="1"/>
+    <col min="13" max="13" width="31.8857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="10" customFormat="1">
+    <row r="1" s="10" customFormat="1" spans="1:13">
       <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
@@ -2019,11 +2498,11 @@
       <c r="L1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:13">
       <c r="A2" s="17" t="s">
         <v>37</v>
       </c>
@@ -2064,7 +2543,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="43.2">
+    <row r="3" ht="45" spans="1:13">
       <c r="A3" s="17" t="s">
         <v>49</v>
       </c>
@@ -2099,7 +2578,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="43.2">
+    <row r="4" ht="45" spans="1:13">
       <c r="A4" s="17" t="s">
         <v>56</v>
       </c>
@@ -2134,7 +2613,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="43.2">
+    <row r="5" ht="45" spans="1:13">
       <c r="A5" s="17" t="s">
         <v>64</v>
       </c>
@@ -2169,7 +2648,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="43.2">
+    <row r="6" ht="45" spans="1:13">
       <c r="A6" s="17" t="s">
         <v>65</v>
       </c>
@@ -2327,7 +2806,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="52.05" customHeight="1">
+    <row r="10" ht="52.05" customHeight="1" spans="1:13">
       <c r="A10" s="17" t="s">
         <v>76</v>
       </c>
@@ -2406,7 +2885,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="28.8">
+    <row r="12" ht="30" spans="1:13">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -2444,7 +2923,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="28.8">
+    <row r="13" ht="30" spans="1:13">
       <c r="A13" t="s">
         <v>89</v>
       </c>
@@ -2482,7 +2961,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="28.8">
+    <row r="14" ht="30" spans="1:13">
       <c r="A14" s="19" t="s">
         <v>91</v>
       </c>
@@ -2515,7 +2994,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -2556,7 +3035,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>104</v>
       </c>
@@ -2594,7 +3073,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>107</v>
       </c>
@@ -2632,7 +3111,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>110</v>
       </c>
@@ -2667,7 +3146,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>112</v>
       </c>
@@ -2828,7 +3307,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:13">
       <c r="A23" s="20" t="s">
         <v>121</v>
       </c>
@@ -2866,7 +3345,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="43.2">
+    <row r="24" ht="45" spans="1:13">
       <c r="A24" s="15" t="s">
         <v>124</v>
       </c>
@@ -2898,7 +3377,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="43.2">
+    <row r="25" ht="45" spans="1:13">
       <c r="A25" s="15" t="s">
         <v>126</v>
       </c>
@@ -2930,7 +3409,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" ht="30" spans="1:14">
       <c r="A26" s="15" t="s">
         <v>129</v>
       </c>
@@ -2974,7 +3453,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" ht="30" spans="1:13">
       <c r="A27" s="15" t="s">
         <v>133</v>
       </c>
@@ -3061,45 +3540,47 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" tooltip="https://www.linkedin.com/in/" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="G2" r:id="rId2" tooltip="https://www.linkedin.com/in/apple bees/" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="G4" r:id="rId3" tooltip="https://www.linkedin.com/in/honey comb" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="G5" r:id="rId4" tooltip="https://www.linkedin.com/in/honey comb" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="G6" r:id="rId5" tooltip="https://www.linkedin.com/in/honey comb" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="G8" r:id="rId6" tooltip="https://www.linkedin.com/in/honey comb" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink ref="G9" r:id="rId7" tooltip="https://www.linkedin.com/in/honey comb" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
-    <hyperlink ref="G10" r:id="rId8" tooltip="https://www.linkedin.com/in/honey comb" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink ref="G11" r:id="rId9" tooltip="https://www.linkedin.com/in/honey comb" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
-    <hyperlink ref="G12" r:id="rId10" tooltip="https://www.linkedin.com/in/honey comb" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
-    <hyperlink ref="G13" r:id="rId11" tooltip="https://www.linkedin.com/in/honey comb" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
-    <hyperlink ref="G15" r:id="rId12" tooltip="https://www.linkedin.com/in/sansacindy" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
-    <hyperlink ref="G16" r:id="rId13" tooltip="https://www.linkedin.com/in/sansacindy" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
-    <hyperlink ref="G17" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
-    <hyperlink ref="G18" r:id="rId15" tooltip="https://www.linkedin.com/in/sansacindy" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
-    <hyperlink ref="G19" r:id="rId16" tooltip="https://www.linkedin.com/in/sansacindy" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
-    <hyperlink ref="G20" r:id="rId17" tooltip="https://linkedin.com/in/apple bees/" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
-    <hyperlink ref="G21" r:id="rId18" tooltip="https://www.linkedin.com/in/apple bees/" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
-    <hyperlink ref="G22" r:id="rId19" tooltip="https://www.linkedin.com/in/sansacindy" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
-    <hyperlink ref="G23" r:id="rId20" tooltip="https://www.linkedin.com/in/sansacindy" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
-    <hyperlink ref="G24" r:id="rId21" tooltip="https://www.linkedin.com/in/sansacindy" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
-    <hyperlink ref="G25" r:id="rId22" tooltip="https://www.linkedin.com/in/sansacindy" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
-    <hyperlink ref="G26" r:id="rId23" tooltip="https://www.linkedin.com/in/sansacindy" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
-    <hyperlink ref="G27" r:id="rId24" tooltip="https://www.linkedin.com/in/sansacindy" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
-    <hyperlink ref="G28" r:id="rId25" tooltip="https://www.linkedin.com/in/apple bees/" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="G3" r:id="rId1" display="https://www.linkedin.com/in/" tooltip="https://www.linkedin.com/in/"/>
+    <hyperlink ref="G2" r:id="rId2" display="https://www.linkedin.com/in/apple bees/" tooltip="https://www.linkedin.com/in/apple bees/"/>
+    <hyperlink ref="G4" r:id="rId2" display="https://www.linkedin.com/in/honey comb" tooltip="https://www.linkedin.com/in/honey comb"/>
+    <hyperlink ref="G5" r:id="rId2" display="https://www.linkedin.com/in/honey comb" tooltip="https://www.linkedin.com/in/honey comb"/>
+    <hyperlink ref="G6" r:id="rId2" display="https://www.linkedin.com/in/honey comb" tooltip="https://www.linkedin.com/in/honey comb"/>
+    <hyperlink ref="G8" r:id="rId2" display="https://www.linkedin.com/in/honey comb" tooltip="https://www.linkedin.com/in/honey comb"/>
+    <hyperlink ref="G9" r:id="rId2" display="https://www.linkedin.com/in/honey comb" tooltip="https://www.linkedin.com/in/honey comb"/>
+    <hyperlink ref="G10" r:id="rId2" display="https://www.linkedin.com/in/honey comb" tooltip="https://www.linkedin.com/in/honey comb"/>
+    <hyperlink ref="G11" r:id="rId2" display="https://www.linkedin.com/in/honey comb" tooltip="https://www.linkedin.com/in/honey comb"/>
+    <hyperlink ref="G12" r:id="rId2" display="https://www.linkedin.com/in/honey comb" tooltip="https://www.linkedin.com/in/honey comb"/>
+    <hyperlink ref="G13" r:id="rId2" display="https://www.linkedin.com/in/honey comb" tooltip="https://www.linkedin.com/in/honey comb"/>
+    <hyperlink ref="G15" r:id="rId3" display="https://www.linkedin.com/in/sansacindy" tooltip="https://www.linkedin.com/in/sansacindy"/>
+    <hyperlink ref="G16" r:id="rId3" display="https://www.linkedin.com/in/sansacindy" tooltip="https://www.linkedin.com/in/sansacindy"/>
+    <hyperlink ref="G17" r:id="rId4" display="https://www.google.com/"/>
+    <hyperlink ref="G18" r:id="rId3" display="https://www.linkedin.com/in/sansacindy" tooltip="https://www.linkedin.com/in/sansacindy"/>
+    <hyperlink ref="G19" r:id="rId3" display="https://www.linkedin.com/in/sansacindy" tooltip="https://www.linkedin.com/in/sansacindy"/>
+    <hyperlink ref="G20" r:id="rId2" display="https://linkedin.com/in/apple bees/" tooltip="https://linkedin.com/in/apple bees/"/>
+    <hyperlink ref="G21" r:id="rId2" display="https://www.linkedin.com/in/apple bees/" tooltip="https://www.linkedin.com/in/apple bees/"/>
+    <hyperlink ref="G22" r:id="rId3" display="https://www.linkedin.com/in/sansacindy" tooltip="https://www.linkedin.com/in/sansacindy"/>
+    <hyperlink ref="G23" r:id="rId3" display="https://www.linkedin.com/in/sansacindy" tooltip="https://www.linkedin.com/in/sansacindy"/>
+    <hyperlink ref="G24" r:id="rId3" display="https://www.linkedin.com/in/sansacindy" tooltip="https://www.linkedin.com/in/sansacindy"/>
+    <hyperlink ref="G25" r:id="rId3" display="https://www.linkedin.com/in/sansacindy" tooltip="https://www.linkedin.com/in/sansacindy"/>
+    <hyperlink ref="G26" r:id="rId3" display="https://www.linkedin.com/in/sansacindy" tooltip="https://www.linkedin.com/in/sansacindy"/>
+    <hyperlink ref="G27" r:id="rId3" display="https://www.linkedin.com/in/sansacindy" tooltip="https://www.linkedin.com/in/sansacindy"/>
+    <hyperlink ref="G28" r:id="rId2" display="https://www.linkedin.com/in/apple bees/" tooltip="https://www.linkedin.com/in/apple bees/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D6"/>
+      <selection activeCell="A1" sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -3182,34 +3663,36 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.8857142857143" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.1047619047619" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.552380952381" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.8857142857143" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.3333333333333" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.4380952380952" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.1047619047619" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="14" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.6640625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.5546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.552380952381" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.6666666666667" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.552380952381" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="10" customFormat="1">
+    <row r="1" s="10" customFormat="1" spans="1:13">
       <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
@@ -3247,7 +3730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.8">
+    <row r="2" ht="30" spans="1:13">
       <c r="A2" s="12" t="s">
         <v>151</v>
       </c>
@@ -3284,36 +3767,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" tooltip="https://www.linkedin.com/in/apple bees/" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="G2" r:id="rId1" display="https://www.linkedin.com/in/apple bees/" tooltip="https://www.linkedin.com/in/apple bees/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="43.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="21.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.88671875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="28.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.4380952380952" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.3333333333333" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.8857142857143" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.6666666666667" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="43.1047619047619" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="21.4380952380952" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.8857142857143" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.1047619047619" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.8857142857143" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.6666666666667" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="28.4380952380952" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="10" customFormat="1">
+    <row r="1" s="10" customFormat="1" spans="1:13">
       <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
@@ -3352,7 +3837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="79.05" customHeight="1">
+    <row r="2" ht="79.05" customHeight="1" spans="1:13">
       <c r="A2" s="12" t="s">
         <v>151</v>
       </c>
@@ -3389,35 +3874,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" tooltip="https://www.linkedin.com/in/apple bees/" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="G2" r:id="rId1" display="https://www.linkedin.com/in/apple bees/" tooltip="https://www.linkedin.com/in/apple bees/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="3" max="3" width="27.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.6666666666667" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="17.3333333333333" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.8857142857143" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="24" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="27.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="34.44140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="42.44140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.1047619047619" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.4380952380952" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.1047619047619" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="27.6666666666667" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="34.4380952380952" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="42.4380952380952" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="10" customFormat="1">
+    <row r="1" s="10" customFormat="1" spans="1:13">
       <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
@@ -3456,7 +3943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="86.4">
+    <row r="2" ht="105" spans="1:13">
       <c r="A2" s="12" t="s">
         <v>151</v>
       </c>
@@ -3493,26 +3980,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" tooltip="https://www.linkedin.com/in/apple bees/" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="G2" r:id="rId1" display="https://www.linkedin.com/in/apple bees/" tooltip="https://www.linkedin.com/in/apple bees/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="13" max="13" width="30.33203125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="30.3333333333333" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="10" customFormat="1">
+    <row r="1" s="10" customFormat="1" spans="1:13">
       <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
@@ -3551,7 +4040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="86.4">
+    <row r="2" ht="105" spans="1:13">
       <c r="A2" s="12" t="s">
         <v>151</v>
       </c>
@@ -3589,32 +4078,34 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="4" max="4" width="22.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.5546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.6666666666667" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.4380952380952" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.552380952381" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.552380952381" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="14" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.88671875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="21.33203125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.552380952381" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.3333333333333" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.4380952380952" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.8857142857143" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="21.3333333333333" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="10" customFormat="1">
+    <row r="1" s="10" customFormat="1" spans="1:13">
       <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
@@ -3653,7 +4144,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="86.4">
+    <row r="2" ht="105" spans="1:13">
       <c r="A2" s="12" t="s">
         <v>151</v>
       </c>
@@ -3690,8 +4181,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" tooltip="https://www.linkedin.com/in/apple bees/" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="G2" r:id="rId1" display="https://www.linkedin.com/in/apple bees/" tooltip="https://www.linkedin.com/in/apple bees/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>